<commit_message>
Update template files for import trips
</commit_message>
<xml_diff>
--- a/angular/src/assets/sampleFiles/ImportGoodsDetailsRequestSampleFile.xlsx
+++ b/angular/src/assets/sampleFiles/ImportGoodsDetailsRequestSampleFile.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25019"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25108"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FE47E08-CCC3-4FDE-8626-4CD5C5B2C690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{447C546C-F389-43DD-91E8-16C5EF6A0EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Trip Reference*</t>
   </si>
@@ -45,6 +44,9 @@
   </si>
   <si>
     <t>Unit Of Measure*</t>
+  </si>
+  <si>
+    <t>Other Unit Of Measure</t>
   </si>
   <si>
     <t>Weight Per Item*</t>
@@ -447,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -461,15 +463,16 @@
     <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -506,69 +509,78 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2">
+        <v>15</v>
+      </c>
+      <c r="H2">
         <v>1000</v>
       </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2">
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2">
         <v>1</v>
       </c>
-      <c r="J2" t="s">
-        <v>16</v>
+      <c r="K2" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3">
+        <v>20</v>
+      </c>
+      <c r="H3">
         <v>1000</v>
       </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3">
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3">
         <v>2</v>
-      </c>
-      <c r="J3" t="s">
-        <v>21</v>
       </c>
       <c r="K3" t="s">
         <v>22</v>
       </c>
-      <c r="L3">
+      <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3">
         <v>431315</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D5" xr:uid="{3E993F42-FD12-40F2-A931-AE21AE1682F6}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F4" xr:uid="{0245E996-BFD8-4815-AC7D-9A1889F15C74}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D5 G2 F2 F3" xr:uid="{3E993F42-FD12-40F2-A931-AE21AE1682F6}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G4 F4" xr:uid="{0245E996-BFD8-4815-AC7D-9A1889F15C74}">
       <formula1>"Litre, Box, Bag, Piece, weight-kg"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
TAC-3045 Convert yes, no to list in imprt from excel
</commit_message>
<xml_diff>
--- a/angular/src/assets/sampleFiles/ImportGoodsDetailsRequestSampleFile.xlsx
+++ b/angular/src/assets/sampleFiles/ImportGoodsDetailsRequestSampleFile.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25113"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{447C546C-F389-43DD-91E8-16C5EF6A0EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F1CAB88-C4F8-44F2-ABC6-19B97ECD3F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -451,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -578,10 +579,13 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D5 G2 F2 F3" xr:uid="{3E993F42-FD12-40F2-A931-AE21AE1682F6}"/>
+  <dataValidations count="3">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D5 G2 F2:F3" xr:uid="{3E993F42-FD12-40F2-A931-AE21AE1682F6}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G4 F4" xr:uid="{0245E996-BFD8-4815-AC7D-9A1889F15C74}">
       <formula1>"Litre, Box, Bag, Piece, weight-kg"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K3" xr:uid="{4B82691A-8AEB-4A18-B507-158BC9660382}">
+      <formula1>"yes,no"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
TAC-3791  Fix validation issues for import shipment excel
</commit_message>
<xml_diff>
--- a/angular/src/assets/sampleFiles/ImportGoodsDetailsRequestSampleFile.xlsx
+++ b/angular/src/assets/sampleFiles/ImportGoodsDetailsRequestSampleFile.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25425"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F1CAB88-C4F8-44F2-ABC6-19B97ECD3F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{69416CD7-783E-4F62-B764-993F5454F843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,78 +27,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t>Trip Reference*</t>
-  </si>
-  <si>
-    <t>Point Reference*</t>
-  </si>
-  <si>
-    <t>Goods Sub Category*</t>
-  </si>
-  <si>
-    <t>Other Goods Sub Category</t>
-  </si>
-  <si>
-    <t>Goods Description*</t>
-  </si>
-  <si>
-    <t>Unit Of Measure*</t>
-  </si>
-  <si>
-    <t>Other Unit Of Measure</t>
-  </si>
-  <si>
-    <t>Weight Per Item*</t>
-  </si>
-  <si>
-    <t>Package Dimensions*</t>
-  </si>
-  <si>
-    <t>Quantity*</t>
-  </si>
-  <si>
-    <t>Is Dangerous Goods?*</t>
-  </si>
-  <si>
-    <t>DangerousGoodType</t>
-  </si>
-  <si>
-    <t>DangerousGoodsCode</t>
-  </si>
-  <si>
-    <t>Fishes</t>
-  </si>
-  <si>
-    <t>sadsad</t>
-  </si>
-  <si>
-    <t>Box</t>
-  </si>
-  <si>
-    <t>50*52</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>water</t>
-  </si>
-  <si>
-    <t>dfdgdf</t>
-  </si>
-  <si>
-    <t>Litre</t>
-  </si>
-  <si>
-    <t>500*600</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Gases</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>Trip Reference* رقم الرحلة</t>
+  </si>
+  <si>
+    <t>Point Reference* رقم نقطة التوصيل</t>
+  </si>
+  <si>
+    <t>Goods Sub Category*  التصنيف الفرعي</t>
+  </si>
+  <si>
+    <t>Other Goods Sub Category   تصنيف فرعي اخر</t>
+  </si>
+  <si>
+    <t>الوزن     * Weight</t>
+  </si>
+  <si>
+    <t>Quantity *    الكمية</t>
+  </si>
+  <si>
+    <t>Unit Of Measure*  وحدة القياس</t>
+  </si>
+  <si>
+    <t>Other Unit Of Measure وحدة ثيلس أخرى</t>
+  </si>
+  <si>
+    <t>الوصف      *Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dimensions الأبعاد</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is Dangerous Goods? بضائع خطرة ؟ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dangerous Good Type تصنيف البضائع الخطرة </t>
+  </si>
+  <si>
+    <t>Dangerous Goods Code كود البضائع الخطرة</t>
   </si>
 </sst>
 </file>
@@ -450,27 +417,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" customWidth="1"/>
+    <col min="4" max="4" width="43.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="34.7109375" customWidth="1"/>
+    <col min="8" max="8" width="34.5703125" customWidth="1"/>
+    <col min="9" max="9" width="24.28515625" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.7109375" customWidth="1"/>
+    <col min="12" max="12" width="44" customWidth="1"/>
+    <col min="13" max="13" width="40.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -514,77 +481,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2">
-        <v>1000</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3">
-        <v>1000</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-      <c r="K3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3">
-        <v>431315</v>
-      </c>
-    </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D5 G2 F2:F3" xr:uid="{3E993F42-FD12-40F2-A931-AE21AE1682F6}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G4 F4" xr:uid="{0245E996-BFD8-4815-AC7D-9A1889F15C74}">
+  <dataValidations count="4">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:F5 H2:I2 G1 K1" xr:uid="{3E993F42-FD12-40F2-A931-AE21AE1682F6}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:I4" xr:uid="{0245E996-BFD8-4815-AC7D-9A1889F15C74}">
       <formula1>"Litre, Box, Bag, Piece, weight-kg"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K3" xr:uid="{4B82691A-8AEB-4A18-B507-158BC9660382}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{670C20C3-B83F-4C6D-9119-46B6C4984B13}">
+      <formula1>"Litre,Box,Bag"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{0F46DDD2-4A96-4EEB-9404-76CBFA796C19}">
       <formula1>"yes,no"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add translation for fields in excel
</commit_message>
<xml_diff>
--- a/angular/src/assets/sampleFiles/ImportGoodsDetailsRequestSampleFile.xlsx
+++ b/angular/src/assets/sampleFiles/ImportGoodsDetailsRequestSampleFile.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25428"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69416CD7-783E-4F62-B764-993F5454F843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D45C470-5AC4-443B-A723-520B48A4A15B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
     <t>Unit Of Measure*  وحدة القياس</t>
   </si>
   <si>
-    <t>Other Unit Of Measure وحدة ثيلس أخرى</t>
+    <t>Other Unit Of Measure وحدة قياس أخرى</t>
   </si>
   <si>
     <t>الوصف      *Description</t>
@@ -419,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -482,8 +482,8 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:F5 H2:I2 G1 K1" xr:uid="{3E993F42-FD12-40F2-A931-AE21AE1682F6}"/>
+  <dataValidations count="5">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1 H2:I2 G1 D2:F5" xr:uid="{3E993F42-FD12-40F2-A931-AE21AE1682F6}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:I4" xr:uid="{0245E996-BFD8-4815-AC7D-9A1889F15C74}">
       <formula1>"Litre, Box, Bag, Piece, weight-kg"</formula1>
     </dataValidation>
@@ -493,6 +493,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{0F46DDD2-4A96-4EEB-9404-76CBFA796C19}">
       <formula1>"yes,no"</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{ABB43B09-613A-4F92-9663-69EE54273E43}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
TAC-3831 Fix enable TMS to import trips and edit lists of sub category in excel file
</commit_message>
<xml_diff>
--- a/angular/src/assets/sampleFiles/ImportGoodsDetailsRequestSampleFile.xlsx
+++ b/angular/src/assets/sampleFiles/ImportGoodsDetailsRequestSampleFile.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25428"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25510"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D45C470-5AC4-443B-A723-520B48A4A15B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{3D45C470-5AC4-443B-A723-520B48A4A15B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7A1F620-CC82-4AF6-A24D-F93052DF2365}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Lists" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>Trip Reference* رقم الرحلة</t>
   </si>
@@ -66,19 +67,113 @@
   </si>
   <si>
     <t>Dangerous Goods Code كود البضائع الخطرة</t>
+  </si>
+  <si>
+    <t>Dry goods</t>
+  </si>
+  <si>
+    <t>Good Sub Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Packed food </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diary product </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beverages </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fresh food </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grains &amp; beans </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Animal food </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Household electronics </t>
+  </si>
+  <si>
+    <t xml:space="preserve">General electronics </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobiles </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Furniture </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Textiles </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cosmetics </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medicine </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medical equipments </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medical consumables </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Petrochemicals - Dry </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Petrochemicals - Liquid </t>
+  </si>
+  <si>
+    <t>Cars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiers </t>
+  </si>
+  <si>
+    <t>Spare parts</t>
+  </si>
+  <si>
+    <t>Lubricants</t>
+  </si>
+  <si>
+    <t>Steel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minerals </t>
+  </si>
+  <si>
+    <t>Chemicals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Others </t>
+  </si>
+  <si>
+    <t>Container</t>
+  </si>
+  <si>
+    <t>Detergents</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -101,8 +196,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -481,9 +577,14 @@
         <v>12</v>
       </c>
     </row>
+    <row r="2" spans="1:13">
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations count="5">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1 H2:I2 G1 D2:F5" xr:uid="{3E993F42-FD12-40F2-A931-AE21AE1682F6}"/>
+  <dataValidations count="4">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1 H2:I2 G1 D2:F5 C1" xr:uid="{3E993F42-FD12-40F2-A931-AE21AE1682F6}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:I4" xr:uid="{0245E996-BFD8-4815-AC7D-9A1889F15C74}">
       <formula1>"Litre, Box, Bag, Piece, weight-kg"</formula1>
     </dataValidation>
@@ -493,8 +594,182 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{0F46DDD2-4A96-4EEB-9404-76CBFA796C19}">
       <formula1>"yes,no"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{ABB43B09-613A-4F92-9663-69EE54273E43}"/>
   </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FED03012-D630-4B09-A7E3-6D9ABD2F1CBB}">
+          <x14:formula1>
+            <xm:f>Lists!A3:A30</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BC5A6A5-BC38-42A1-9973-EC3D76667F24}">
+  <dimension ref="A1:A29"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TAC-3804  Fix allow carrier saas to import trip , edit excel files
</commit_message>
<xml_diff>
--- a/angular/src/assets/sampleFiles/ImportGoodsDetailsRequestSampleFile.xlsx
+++ b/angular/src/assets/sampleFiles/ImportGoodsDetailsRequestSampleFile.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25510"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{3D45C470-5AC4-443B-A723-520B48A4A15B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7A1F620-CC82-4AF6-A24D-F93052DF2365}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{485CF65A-B12C-45A8-B8E7-8A6FD892300D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Trip Reference* رقم الرحلة</t>
   </si>
@@ -69,82 +69,82 @@
     <t>Dangerous Goods Code كود البضائع الخطرة</t>
   </si>
   <si>
+    <t>Good Sub Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Packed food </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diary product </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beverages </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fresh food </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grains &amp; beans </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Animal food </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Household electronics </t>
+  </si>
+  <si>
+    <t xml:space="preserve">General electronics </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobiles </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Furniture </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Textiles </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cosmetics </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medicine </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medical equipments </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medical consumables </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Petrochemicals - Dry </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Petrochemicals - Liquid </t>
+  </si>
+  <si>
+    <t>Cars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiers </t>
+  </si>
+  <si>
+    <t>Spare parts</t>
+  </si>
+  <si>
+    <t>Lubricants</t>
+  </si>
+  <si>
+    <t>Steel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minerals </t>
+  </si>
+  <si>
+    <t>Chemicals</t>
+  </si>
+  <si>
     <t>Dry goods</t>
-  </si>
-  <si>
-    <t>Good Sub Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Packed food </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diary product </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beverages </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fresh food </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grains &amp; beans </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Animal food </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Household electronics </t>
-  </si>
-  <si>
-    <t xml:space="preserve">General electronics </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mobiles </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Furniture </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Textiles </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cosmetics </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medicine </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medical equipments </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medical consumables </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Petrochemicals - Dry </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Petrochemicals - Liquid </t>
-  </si>
-  <si>
-    <t>Cars</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiers </t>
-  </si>
-  <si>
-    <t>Spare parts</t>
-  </si>
-  <si>
-    <t>Lubricants</t>
-  </si>
-  <si>
-    <t>Steel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minerals </t>
-  </si>
-  <si>
-    <t>Chemicals</t>
   </si>
   <si>
     <t xml:space="preserve">Others </t>
@@ -513,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -577,22 +577,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1 H2:I2 G1 D2:F5 C1" xr:uid="{3E993F42-FD12-40F2-A931-AE21AE1682F6}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1 H2:I2 C1 D2:F5 G1" xr:uid="{3E993F42-FD12-40F2-A931-AE21AE1682F6}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:I4" xr:uid="{0245E996-BFD8-4815-AC7D-9A1889F15C74}">
       <formula1>"Litre, Box, Bag, Piece, weight-kg"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{670C20C3-B83F-4C6D-9119-46B6C4984B13}">
-      <formula1>"Litre,Box,Bag"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{0F46DDD2-4A96-4EEB-9404-76CBFA796C19}">
       <formula1>"yes,no"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{D608E88D-6FCE-4724-B546-F61EC030AF53}">
+      <formula1>"Litre,Box,Bag,Piece,Weight -KG,Pallets,Container,Others"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -626,132 +621,132 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:1">

</xml_diff>

<commit_message>
TAC-3844  Fix edit texts in import trips excel files
</commit_message>
<xml_diff>
--- a/angular/src/assets/sampleFiles/ImportGoodsDetailsRequestSampleFile.xlsx
+++ b/angular/src/assets/sampleFiles/ImportGoodsDetailsRequestSampleFile.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25510"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{485CF65A-B12C-45A8-B8E7-8A6FD892300D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GF\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E73DAF3B-DBB6-49A9-88D0-1D12F764313D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,46 +32,182 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Azhar Safi</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{AE294ADA-A3D7-4E8B-A70A-F0AB0E148242}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Here you should add the same refrance number as in the trips details files</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{59334700-129C-471E-8F94-0F3A38631FE4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Please select one from the list</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{E7E31312-5664-4924-B035-772047B5F2A3}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Please fill this cell only if the goods sub-category is "Others"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{16E6A3DE-90E5-4430-96BF-F567751126B7}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Weight/item
+KG</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{229A9DD0-DABD-460C-AEA0-849FF3C20AC1}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Please select one from the list</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{03B81F7C-43CB-4478-AF89-5E06ED0E10A5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Please fill this cell only if the UOM is "Others"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{84E5AEDD-91D1-4BA8-81F2-B232B967C179}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">Dimintions of the UOM </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{D2370F9D-CCDD-4D29-969A-AE9A1909C73B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">If the goods is dangerous please select yes </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
-    <t>Trip Reference* رقم الرحلة</t>
-  </si>
-  <si>
-    <t>Point Reference* رقم نقطة التوصيل</t>
-  </si>
-  <si>
-    <t>Goods Sub Category*  التصنيف الفرعي</t>
-  </si>
-  <si>
-    <t>Other Goods Sub Category   تصنيف فرعي اخر</t>
-  </si>
-  <si>
-    <t>الوزن     * Weight</t>
-  </si>
-  <si>
-    <t>Quantity *    الكمية</t>
-  </si>
-  <si>
-    <t>Unit Of Measure*  وحدة القياس</t>
-  </si>
-  <si>
-    <t>Other Unit Of Measure وحدة قياس أخرى</t>
-  </si>
-  <si>
-    <t>الوصف      *Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dimensions الأبعاد</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is Dangerous Goods? بضائع خطرة ؟ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dangerous Good Type تصنيف البضائع الخطرة </t>
-  </si>
-  <si>
-    <t>Dangerous Goods Code كود البضائع الخطرة</t>
+    <t>Trip Reference No * 
+الرقم المرجعي للرحلة</t>
+  </si>
+  <si>
+    <t>Point Reference No*
+الرقم المرجعي لنقطة الوصول</t>
+  </si>
+  <si>
+    <t>Goods Sub Category*
+نوع البضاعة</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goods details
+تفاصيل البضاعة   </t>
+  </si>
+  <si>
+    <t>Weight *
+الوزن</t>
+  </si>
+  <si>
+    <t>QTY*
+الكمية</t>
+  </si>
+  <si>
+    <t>UON*
+وحدة القياس</t>
+  </si>
+  <si>
+    <t>UOM description
+وحدة القياس</t>
+  </si>
+  <si>
+    <t>Goods description *
+وصف البضاعة</t>
+  </si>
+  <si>
+    <t>Dimensions
+الأبعاد</t>
+  </si>
+  <si>
+    <t>Is Dangerous Goods?
+بضائع خطرة ؟</t>
+  </si>
+  <si>
+    <t>Dangerous goods type
+نوع البضائع الخطرة</t>
+  </si>
+  <si>
+    <t>Dangerous Goods Code
+رمز البضائع الخطرة</t>
   </si>
   <si>
     <t>Good Sub Category</t>
@@ -160,7 +301,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,11 +310,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF444444"/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -184,7 +337,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -192,13 +345,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,89 +688,118 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" customWidth="1"/>
-    <col min="4" max="4" width="43.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="34.7109375" customWidth="1"/>
-    <col min="8" max="8" width="34.5703125" customWidth="1"/>
-    <col min="9" max="9" width="24.28515625" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" customWidth="1"/>
-    <col min="12" max="12" width="44" customWidth="1"/>
-    <col min="13" max="13" width="40.140625" customWidth="1"/>
+    <col min="1" max="2" width="32.85546875" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" customWidth="1"/>
+    <col min="4" max="4" width="45.42578125" customWidth="1"/>
+    <col min="5" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" customWidth="1"/>
+    <col min="8" max="8" width="34.85546875" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" customWidth="1"/>
+    <col min="10" max="10" width="32.42578125" customWidth="1"/>
+    <col min="11" max="11" width="35.42578125" customWidth="1"/>
+    <col min="12" max="12" width="43.28515625" customWidth="1"/>
+    <col min="13" max="13" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" s="4" customFormat="1" ht="25.5">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" s="4" customFormat="1" ht="11.25">
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:14" s="4" customFormat="1" ht="11.25"/>
+    <row r="4" spans="1:14" s="4" customFormat="1" ht="11.25"/>
+    <row r="5" spans="1:14" s="4" customFormat="1" ht="11.25"/>
+    <row r="6" spans="1:14" s="4" customFormat="1" ht="11.25"/>
+    <row r="7" spans="1:14" s="4" customFormat="1" ht="11.25"/>
+    <row r="8" spans="1:14" s="4" customFormat="1" ht="11.25"/>
+    <row r="9" spans="1:14" s="4" customFormat="1" ht="11.25"/>
+    <row r="10" spans="1:14" s="4" customFormat="1" ht="11.25"/>
+    <row r="11" spans="1:14" s="4" customFormat="1" ht="11.25"/>
+    <row r="12" spans="1:14" s="4" customFormat="1" ht="11.25"/>
+    <row r="13" spans="1:14" s="4" customFormat="1" ht="11.25"/>
+    <row r="14" spans="1:14" s="4" customFormat="1" ht="11.25"/>
+    <row r="15" spans="1:14" s="4" customFormat="1" ht="11.25"/>
+    <row r="16" spans="1:14" s="4" customFormat="1" ht="11.25"/>
+    <row r="17" s="4" customFormat="1" ht="11.25"/>
+    <row r="18" s="4" customFormat="1" ht="11.25"/>
+    <row r="19" s="4" customFormat="1" ht="11.25"/>
+    <row r="20" s="4" customFormat="1" ht="11.25"/>
+    <row r="21" s="4" customFormat="1" ht="11.25"/>
+    <row r="22" s="4" customFormat="1" ht="11.25"/>
+    <row r="23" s="4" customFormat="1" ht="11.25"/>
+    <row r="24" s="4" customFormat="1" ht="11.25"/>
+    <row r="25" s="4" customFormat="1" ht="11.25"/>
+    <row r="26" s="4" customFormat="1" ht="11.25"/>
+    <row r="27" s="4" customFormat="1" ht="11.25"/>
+    <row r="28" s="4" customFormat="1" ht="11.25"/>
+    <row r="29" s="4" customFormat="1" ht="11.25"/>
+    <row r="30" s="4" customFormat="1" ht="11.25"/>
+    <row r="31" customFormat="1"/>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1 H2:I2 C1 D2:F5 G1" xr:uid="{3E993F42-FD12-40F2-A931-AE21AE1682F6}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:I4" xr:uid="{0245E996-BFD8-4815-AC7D-9A1889F15C74}">
-      <formula1>"Litre, Box, Bag, Piece, weight-kg"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{0F46DDD2-4A96-4EEB-9404-76CBFA796C19}">
+  <dataValidations count="3">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H4 D2:D5" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"yes,no"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{D608E88D-6FCE-4724-B546-F61EC030AF53}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{D0492BDA-BD97-4018-B6DF-4E6DF538AADD}">
       <formula1>"Litre,Box,Bag,Piece,Weight -KG,Pallets,Container,Others"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FED03012-D630-4B09-A7E3-6D9ABD2F1CBB}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ED6871D4-4BED-42BA-9961-52B399406C1F}">
           <x14:formula1>
             <xm:f>Lists!A3:A30</xm:f>
           </x14:formula1>
@@ -607,16 +812,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BC5A6A5-BC38-42A1-9973-EC3D76667F24}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8FE615C-AA91-400F-8BB4-3BC25ED64E47}">
   <dimension ref="A1:A29"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -625,7 +830,7 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>